<commit_message>
Bound propagation and standard form for spicy matrix
</commit_message>
<xml_diff>
--- a/bounds_output.xlsx
+++ b/bounds_output.xlsx
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Infinite</t>
+          <t>Finite</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Infinite</t>
+          <t>Finite</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Infinite</t>
+          <t>Finite</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Infinite</t>
+          <t>Finite</t>
         </is>
       </c>
     </row>

</xml_diff>